<commit_message>
changed the activities nama and code for getting the email address from config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -177,6 +177,18 @@
   </si>
   <si>
     <t>https://jobs.telegraph.co.uk</t>
+  </si>
+  <si>
+    <t>SenderMailId</t>
+  </si>
+  <si>
+    <t>SenderMailId_Password</t>
+  </si>
+  <si>
+    <t>uipathtest90@gmail.com</t>
+  </si>
+  <si>
+    <t>uipath@90</t>
   </si>
 </sst>
 </file>
@@ -510,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1591,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1819,8 +1831,22 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2797,6 +2823,9 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B24" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>